<commit_message>
upload UI design by Leo Feb 16,2015
</commit_message>
<xml_diff>
--- a/design/database design specification.xlsx
+++ b/design/database design specification.xlsx
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H183"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B183" sqref="B183"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
upload UI design documents by Leo Feb 22,2015
</commit_message>
<xml_diff>
--- a/design/database design specification.xlsx
+++ b/design/database design specification.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="126">
   <si>
     <t>NAME</t>
   </si>
@@ -387,6 +387,37 @@
   </si>
   <si>
     <t>Primary Key. Parameter name.</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>true- default account; false- not default account;</t>
+  </si>
+  <si>
+    <t>bankid</t>
+  </si>
+  <si>
+    <t>int unsigned</t>
+  </si>
+  <si>
+    <t>T_Bank</t>
+  </si>
+  <si>
+    <t>Primary Key. Bank ID.</t>
+  </si>
+  <si>
+    <t>paypal user password</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>paypal user name</t>
+  </si>
+  <si>
+    <t>user status:
+0-active; 1- pending; 2-</t>
   </si>
 </sst>
 </file>
@@ -874,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H183"/>
+  <dimension ref="B2:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1179,13 +1210,19 @@
       <c r="G24" s="10"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="2:8">
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
+    <row r="25" spans="2:8" ht="30">
+      <c r="C25" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11"/>
       <c r="G25" s="11"/>
-      <c r="H25" s="4"/>
+      <c r="H25" s="4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1">
       <c r="C26" s="13"/>
@@ -2585,8 +2622,12 @@
       <c r="H159" s="8"/>
     </row>
     <row r="160" spans="2:8">
-      <c r="C160" s="3"/>
-      <c r="D160" s="4"/>
+      <c r="C160" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="E160" s="5"/>
       <c r="F160" s="6"/>
       <c r="G160" s="5"/>
@@ -2631,204 +2672,338 @@
       </c>
     </row>
     <row r="164" spans="2:8">
-      <c r="C164" s="3"/>
-      <c r="D164" s="4"/>
+      <c r="C164" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="E164" s="5"/>
       <c r="F164" s="6"/>
       <c r="G164" s="5"/>
-      <c r="H164" s="4"/>
-    </row>
-    <row r="165" spans="2:8" ht="15.75" thickBot="1">
-      <c r="C165" s="13"/>
-      <c r="D165" s="12"/>
-      <c r="E165" s="14"/>
-      <c r="F165" s="14"/>
-      <c r="G165" s="14"/>
-      <c r="H165" s="12"/>
-    </row>
-    <row r="166" spans="2:8">
-      <c r="C166" s="16"/>
-      <c r="D166" s="24"/>
-      <c r="E166" s="25"/>
-      <c r="F166" s="25"/>
-      <c r="G166" s="25"/>
-      <c r="H166" s="24"/>
-    </row>
-    <row r="168" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B168" s="21">
+      <c r="H164" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="165" spans="2:8">
+      <c r="C165" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D165" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E165" s="9"/>
+      <c r="F165" s="10"/>
+      <c r="G165" s="10"/>
+      <c r="H165" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="166" spans="2:8" ht="30">
+      <c r="C166" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E166" s="5"/>
+      <c r="F166" s="6"/>
+      <c r="G166" s="5"/>
+      <c r="H166" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="167" spans="2:8" ht="15.75" thickBot="1">
+      <c r="C167" s="13"/>
+      <c r="D167" s="12"/>
+      <c r="E167" s="14"/>
+      <c r="F167" s="14"/>
+      <c r="G167" s="14"/>
+      <c r="H167" s="12"/>
+    </row>
+    <row r="168" spans="2:8">
+      <c r="C168" s="16"/>
+      <c r="D168" s="24"/>
+      <c r="E168" s="25"/>
+      <c r="F168" s="25"/>
+      <c r="G168" s="25"/>
+      <c r="H168" s="24"/>
+    </row>
+    <row r="169" spans="2:8">
+      <c r="C169" s="16"/>
+      <c r="D169" s="24"/>
+      <c r="E169" s="25"/>
+      <c r="F169" s="25"/>
+      <c r="G169" s="25"/>
+      <c r="H169" s="24"/>
+    </row>
+    <row r="170" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B170" s="21">
+        <v>11</v>
+      </c>
+      <c r="C170" s="22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="171" spans="2:8" ht="15.75" thickBot="1">
+      <c r="C171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F171" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G171" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H171" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="172" spans="2:8">
+      <c r="C172" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D172" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E172" s="18"/>
+      <c r="F172" s="19"/>
+      <c r="G172" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H172" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="173" spans="2:8">
+      <c r="C173" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D173" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C168" s="22" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="169" spans="2:8" ht="15.75" thickBot="1">
-      <c r="C169" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D169" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E169" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F169" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G169" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H169" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="170" spans="2:8">
-      <c r="C170" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D170" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E170" s="18"/>
-      <c r="F170" s="19"/>
-      <c r="G170" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H170" s="16" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="171" spans="2:8">
-      <c r="C171" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D171" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E171" s="5"/>
-      <c r="F171" s="6"/>
-      <c r="G171" s="5"/>
-      <c r="H171" s="4"/>
-    </row>
-    <row r="172" spans="2:8">
-      <c r="C172" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="D172" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E172" s="9"/>
-      <c r="F172" s="10"/>
-      <c r="G172" s="10"/>
-      <c r="H172" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="173" spans="2:8">
-      <c r="C173" s="3"/>
-      <c r="D173" s="4"/>
       <c r="E173" s="5"/>
       <c r="F173" s="6"/>
       <c r="G173" s="5"/>
       <c r="H173" s="4"/>
     </row>
-    <row r="174" spans="2:8" ht="15.75" thickBot="1">
-      <c r="C174" s="13"/>
-      <c r="D174" s="12"/>
-      <c r="E174" s="14"/>
-      <c r="F174" s="14"/>
-      <c r="G174" s="14"/>
-      <c r="H174" s="12"/>
-    </row>
-    <row r="177" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B177" s="21">
-        <v>14</v>
-      </c>
-      <c r="C177" s="22" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="178" spans="2:8" ht="15.75" thickBot="1">
-      <c r="C178" s="1" t="s">
+    <row r="174" spans="2:8">
+      <c r="C174" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D174" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E174" s="9"/>
+      <c r="F174" s="10"/>
+      <c r="G174" s="10"/>
+      <c r="H174" s="8"/>
+    </row>
+    <row r="175" spans="2:8">
+      <c r="C175" s="3"/>
+      <c r="D175" s="4"/>
+      <c r="E175" s="5"/>
+      <c r="F175" s="6"/>
+      <c r="G175" s="5"/>
+      <c r="H175" s="4"/>
+    </row>
+    <row r="176" spans="2:8" ht="15.75" thickBot="1">
+      <c r="C176" s="13"/>
+      <c r="D176" s="12"/>
+      <c r="E176" s="14"/>
+      <c r="F176" s="14"/>
+      <c r="G176" s="14"/>
+      <c r="H176" s="12"/>
+    </row>
+    <row r="177" spans="2:8">
+      <c r="C177" s="16"/>
+      <c r="D177" s="24"/>
+      <c r="E177" s="25"/>
+      <c r="F177" s="25"/>
+      <c r="G177" s="25"/>
+      <c r="H177" s="24"/>
+    </row>
+    <row r="179" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B179" s="21">
+        <v>13</v>
+      </c>
+      <c r="C179" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="180" spans="2:8" ht="15.75" thickBot="1">
+      <c r="C180" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D178" s="1" t="s">
+      <c r="D180" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E178" s="2" t="s">
+      <c r="E180" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F178" s="2" t="s">
+      <c r="F180" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G178" s="2" t="s">
+      <c r="G180" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H178" s="1" t="s">
+      <c r="H180" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="2:8">
-      <c r="C179" s="17" t="s">
+    <row r="181" spans="2:8">
+      <c r="C181" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D179" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E179" s="18"/>
-      <c r="F179" s="19"/>
-      <c r="G179" s="18" t="s">
+      <c r="D181" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E181" s="18"/>
+      <c r="F181" s="19"/>
+      <c r="G181" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="H179" s="16" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="180" spans="2:8">
-      <c r="C180" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="D180" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E180" s="5"/>
-      <c r="F180" s="6"/>
-      <c r="G180" s="5"/>
-      <c r="H180" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="181" spans="2:8">
-      <c r="C181" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D181" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E181" s="9"/>
-      <c r="F181" s="10"/>
-      <c r="G181" s="10"/>
-      <c r="H181" s="8"/>
+      <c r="H181" s="16" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="182" spans="2:8">
       <c r="C182" s="3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>114</v>
+        <v>13</v>
       </c>
       <c r="E182" s="5"/>
       <c r="F182" s="6"/>
       <c r="G182" s="5"/>
       <c r="H182" s="4"/>
     </row>
-    <row r="183" spans="2:8" ht="15.75" thickBot="1">
-      <c r="C183" s="13"/>
-      <c r="D183" s="12"/>
-      <c r="E183" s="14"/>
-      <c r="F183" s="14"/>
-      <c r="G183" s="14"/>
-      <c r="H183" s="12"/>
+    <row r="183" spans="2:8">
+      <c r="C183" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D183" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E183" s="9"/>
+      <c r="F183" s="10"/>
+      <c r="G183" s="10"/>
+      <c r="H183" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="184" spans="2:8">
+      <c r="C184" s="3"/>
+      <c r="D184" s="4"/>
+      <c r="E184" s="5"/>
+      <c r="F184" s="6"/>
+      <c r="G184" s="5"/>
+      <c r="H184" s="4"/>
+    </row>
+    <row r="185" spans="2:8" ht="15.75" thickBot="1">
+      <c r="C185" s="13"/>
+      <c r="D185" s="12"/>
+      <c r="E185" s="14"/>
+      <c r="F185" s="14"/>
+      <c r="G185" s="14"/>
+      <c r="H185" s="12"/>
+    </row>
+    <row r="188" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B188" s="21">
+        <v>14</v>
+      </c>
+      <c r="C188" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="189" spans="2:8" ht="15.75" thickBot="1">
+      <c r="C189" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F189" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G189" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H189" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="190" spans="2:8">
+      <c r="C190" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D190" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E190" s="18"/>
+      <c r="F190" s="19"/>
+      <c r="G190" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H190" s="16" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="191" spans="2:8">
+      <c r="C191" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E191" s="5"/>
+      <c r="F191" s="6"/>
+      <c r="G191" s="5"/>
+      <c r="H191" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="192" spans="2:8">
+      <c r="C192" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D192" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="E192" s="9"/>
+      <c r="F192" s="10"/>
+      <c r="G192" s="10"/>
+      <c r="H192" s="8"/>
+    </row>
+    <row r="193" spans="3:8">
+      <c r="C193" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E193" s="5"/>
+      <c r="F193" s="6"/>
+      <c r="G193" s="5"/>
+      <c r="H193" s="4"/>
+    </row>
+    <row r="194" spans="3:8" ht="15.75" thickBot="1">
+      <c r="C194" s="13"/>
+      <c r="D194" s="12"/>
+      <c r="E194" s="14"/>
+      <c r="F194" s="14"/>
+      <c r="G194" s="14"/>
+      <c r="H194" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
upload new design documentation by Leo Feb 23,2015
</commit_message>
<xml_diff>
--- a/design/database design specification.xlsx
+++ b/design/database design specification.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="128">
   <si>
     <t>NAME</t>
   </si>
@@ -418,6 +418,12 @@
   <si>
     <t>user status:
 0-active; 1- pending; 2-</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Male; Female</t>
   </si>
 </sst>
 </file>
@@ -907,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1225,12 +1231,18 @@
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1">
-      <c r="C26" s="13"/>
-      <c r="D26" s="12"/>
+      <c r="C26" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>105</v>
+      </c>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
-      <c r="H26" s="12"/>
+      <c r="H26" s="12" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="27" spans="2:8">
       <c r="C27" s="15" t="s">

</xml_diff>

<commit_message>
update by leo March 07,2015
</commit_message>
<xml_diff>
--- a/design/database design specification.xlsx
+++ b/design/database design specification.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="130">
   <si>
     <t>NAME</t>
   </si>
@@ -424,6 +424,12 @@
   </si>
   <si>
     <t>Male; Female</t>
+  </si>
+  <si>
+    <t>min_bv</t>
+  </si>
+  <si>
+    <t>minimum BV</t>
   </si>
 </sst>
 </file>
@@ -913,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1321,43 +1327,49 @@
     </row>
     <row r="34" spans="2:8">
       <c r="C34" s="3" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" s="5">
-        <v>0</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="E34" s="5"/>
       <c r="F34" s="6"/>
       <c r="G34" s="5"/>
       <c r="H34" s="4" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="2:8">
       <c r="C35" s="7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" s="9" t="b">
+        <v>6</v>
+      </c>
+      <c r="E35" s="9">
         <v>0</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="2:8">
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="11"/>
+      <c r="C36" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="11" t="b">
+        <v>0</v>
+      </c>
       <c r="F36" s="11"/>
       <c r="G36" s="11"/>
-      <c r="H36" s="4"/>
+      <c r="H36" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="37" spans="2:8" ht="15.75" thickBot="1">
       <c r="C37" s="13"/>

</xml_diff>

<commit_message>
create spring and hibernate cfg
</commit_message>
<xml_diff>
--- a/design/database design specification.xlsx
+++ b/design/database design specification.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25516"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="2820" yWindow="1140" windowWidth="22020" windowHeight="13960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="129">
   <si>
     <t>NAME</t>
   </si>
@@ -425,12 +430,15 @@
   <si>
     <t>Male; Female</t>
   </si>
+  <si>
+    <t>?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,7 +552,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -615,6 +623,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -910,25 +924,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="20"/>
+    <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.5" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1">
+    <row r="2" spans="2:8" ht="15" thickBot="1">
       <c r="B2" s="21">
         <v>1</v>
       </c>
@@ -936,7 +950,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1">
+    <row r="3" spans="2:8" ht="15" thickBot="1">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
@@ -987,7 +1001,7 @@
       </c>
     </row>
     <row r="6" spans="2:8">
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="26" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="8" t="s">
@@ -1145,7 +1159,7 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="2:8">
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -1193,7 +1207,7 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="2:8">
-      <c r="C23" s="3" t="s">
+      <c r="C23" s="23" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -1216,7 +1230,7 @@
       <c r="G24" s="10"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="2:8" ht="30">
+    <row r="25" spans="2:8" ht="28">
       <c r="C25" s="3" t="s">
         <v>84</v>
       </c>
@@ -1230,7 +1244,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="15.75" thickBot="1">
+    <row r="26" spans="2:8" ht="15" thickBot="1">
       <c r="C26" s="13" t="s">
         <v>126</v>
       </c>
@@ -1249,7 +1263,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="15.75" thickBot="1">
+    <row r="29" spans="2:8" ht="15" thickBot="1">
       <c r="B29" s="21">
         <v>2</v>
       </c>
@@ -1257,7 +1271,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="15.75" thickBot="1">
+    <row r="30" spans="2:8" ht="15" thickBot="1">
       <c r="C30" s="1" t="s">
         <v>0</v>
       </c>
@@ -1294,7 +1308,10 @@
       </c>
     </row>
     <row r="32" spans="2:8">
-      <c r="C32" s="3" t="s">
+      <c r="B32" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C32" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D32" s="4" t="s">
@@ -1359,7 +1376,7 @@
       <c r="G36" s="11"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="2:8" ht="15.75" thickBot="1">
+    <row r="37" spans="2:8" ht="15" thickBot="1">
       <c r="C37" s="13"/>
       <c r="D37" s="12"/>
       <c r="E37" s="14"/>
@@ -1367,7 +1384,7 @@
       <c r="G37" s="14"/>
       <c r="H37" s="12"/>
     </row>
-    <row r="40" spans="2:8" ht="15.75" thickBot="1">
+    <row r="40" spans="2:8" ht="15" thickBot="1">
       <c r="B40" s="21">
         <v>3</v>
       </c>
@@ -1375,7 +1392,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="15.75" thickBot="1">
+    <row r="41" spans="2:8" ht="15" thickBot="1">
       <c r="C41" s="1" t="s">
         <v>0</v>
       </c>
@@ -1438,7 +1455,7 @@
       <c r="H44" s="8"/>
     </row>
     <row r="45" spans="2:8">
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D45" s="4" t="s">
@@ -1486,7 +1503,7 @@
       <c r="H48" s="8"/>
     </row>
     <row r="49" spans="2:8">
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="23" t="s">
         <v>63</v>
       </c>
       <c r="D49" s="4" t="s">
@@ -1497,7 +1514,7 @@
       <c r="G49" s="11"/>
       <c r="H49" s="4"/>
     </row>
-    <row r="50" spans="2:8" ht="15.75" thickBot="1">
+    <row r="50" spans="2:8" ht="15" thickBot="1">
       <c r="C50" s="13"/>
       <c r="D50" s="12"/>
       <c r="E50" s="14"/>
@@ -1505,7 +1522,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="12"/>
     </row>
-    <row r="53" spans="2:8" ht="15.75" thickBot="1">
+    <row r="53" spans="2:8" ht="15" thickBot="1">
       <c r="B53" s="21">
         <v>4</v>
       </c>
@@ -1513,7 +1530,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="15.75" thickBot="1">
+    <row r="54" spans="2:8" ht="15" thickBot="1">
       <c r="C54" s="1" t="s">
         <v>0</v>
       </c>
@@ -1552,7 +1569,7 @@
       </c>
     </row>
     <row r="56" spans="2:8">
-      <c r="C56" s="3" t="s">
+      <c r="C56" s="23" t="s">
         <v>57</v>
       </c>
       <c r="D56" s="4" t="s">
@@ -1583,7 +1600,7 @@
       <c r="G58" s="11"/>
       <c r="H58" s="4"/>
     </row>
-    <row r="59" spans="2:8" ht="15.75" thickBot="1">
+    <row r="59" spans="2:8" ht="15" thickBot="1">
       <c r="C59" s="13"/>
       <c r="D59" s="12"/>
       <c r="E59" s="14"/>
@@ -1591,7 +1608,7 @@
       <c r="G59" s="14"/>
       <c r="H59" s="12"/>
     </row>
-    <row r="62" spans="2:8" ht="15.75" thickBot="1">
+    <row r="62" spans="2:8" ht="15" thickBot="1">
       <c r="B62" s="21">
         <v>5</v>
       </c>
@@ -1599,7 +1616,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="63" spans="2:8" ht="15.75" thickBot="1">
+    <row r="63" spans="2:8" ht="15" thickBot="1">
       <c r="C63" s="1" t="s">
         <v>0</v>
       </c>
@@ -1665,7 +1682,7 @@
       <c r="G67" s="11"/>
       <c r="H67" s="4"/>
     </row>
-    <row r="68" spans="2:8" ht="15.75" thickBot="1">
+    <row r="68" spans="2:8" ht="15" thickBot="1">
       <c r="C68" s="13"/>
       <c r="D68" s="12"/>
       <c r="E68" s="14"/>
@@ -1673,7 +1690,7 @@
       <c r="G68" s="14"/>
       <c r="H68" s="12"/>
     </row>
-    <row r="71" spans="2:8" ht="15.75" thickBot="1">
+    <row r="71" spans="2:8" ht="15" thickBot="1">
       <c r="B71" s="21">
         <v>6</v>
       </c>
@@ -1681,7 +1698,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="15.75" thickBot="1">
+    <row r="72" spans="2:8" ht="15" thickBot="1">
       <c r="C72" s="1" t="s">
         <v>0</v>
       </c>
@@ -1718,7 +1735,7 @@
       </c>
     </row>
     <row r="74" spans="2:8">
-      <c r="C74" s="3" t="s">
+      <c r="C74" s="23" t="s">
         <v>58</v>
       </c>
       <c r="D74" s="4" t="s">
@@ -1744,7 +1761,7 @@
       <c r="H75" s="8"/>
     </row>
     <row r="76" spans="2:8">
-      <c r="C76" s="3" t="s">
+      <c r="C76" s="23" t="s">
         <v>57</v>
       </c>
       <c r="D76" s="4" t="s">
@@ -1775,7 +1792,7 @@
       <c r="G78" s="11"/>
       <c r="H78" s="4"/>
     </row>
-    <row r="79" spans="2:8" ht="15.75" thickBot="1">
+    <row r="79" spans="2:8" ht="15" thickBot="1">
       <c r="C79" s="13"/>
       <c r="D79" s="12"/>
       <c r="E79" s="14"/>
@@ -1783,7 +1800,7 @@
       <c r="G79" s="14"/>
       <c r="H79" s="12"/>
     </row>
-    <row r="82" spans="2:8" ht="15.75" thickBot="1">
+    <row r="82" spans="2:8" ht="15" thickBot="1">
       <c r="B82" s="21">
         <v>7</v>
       </c>
@@ -1791,7 +1808,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="2:8" ht="15.75" thickBot="1">
+    <row r="83" spans="2:8" ht="15" thickBot="1">
       <c r="C83" s="1" t="s">
         <v>0</v>
       </c>
@@ -1842,7 +1859,7 @@
       </c>
     </row>
     <row r="86" spans="2:8">
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="26" t="s">
         <v>58</v>
       </c>
       <c r="D86" s="8" t="s">
@@ -1856,7 +1873,7 @@
       </c>
     </row>
     <row r="87" spans="2:8">
-      <c r="C87" s="3" t="s">
+      <c r="C87" s="23" t="s">
         <v>32</v>
       </c>
       <c r="D87" s="4" t="s">
@@ -1868,7 +1885,7 @@
       <c r="H87" s="4"/>
     </row>
     <row r="88" spans="2:8">
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="26" t="s">
         <v>99</v>
       </c>
       <c r="D88" s="8" t="s">
@@ -1893,15 +1910,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="90" spans="2:8" ht="15.75" thickBot="1">
-      <c r="C90" s="13"/>
+    <row r="90" spans="2:8" ht="15" thickBot="1">
+      <c r="C90" s="27" t="s">
+        <v>57</v>
+      </c>
       <c r="D90" s="12"/>
       <c r="E90" s="14"/>
       <c r="F90" s="14"/>
       <c r="G90" s="14"/>
       <c r="H90" s="12"/>
     </row>
-    <row r="93" spans="2:8" ht="15.75" thickBot="1">
+    <row r="93" spans="2:8" ht="15" thickBot="1">
       <c r="B93" s="21">
         <v>8</v>
       </c>
@@ -1909,7 +1928,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="94" spans="2:8" ht="15.75" thickBot="1">
+    <row r="94" spans="2:8" ht="15" thickBot="1">
       <c r="C94" s="1" t="s">
         <v>0</v>
       </c>
@@ -1972,7 +1991,7 @@
       <c r="H97" s="8"/>
     </row>
     <row r="98" spans="2:8">
-      <c r="C98" s="3" t="s">
+      <c r="C98" s="23" t="s">
         <v>57</v>
       </c>
       <c r="D98" s="4" t="s">
@@ -2016,7 +2035,7 @@
       <c r="H101" s="8"/>
     </row>
     <row r="102" spans="2:8">
-      <c r="C102" s="3" t="s">
+      <c r="C102" s="23" t="s">
         <v>54</v>
       </c>
       <c r="D102" s="4" t="s">
@@ -2099,7 +2118,7 @@
       <c r="G108" s="11"/>
       <c r="H108" s="4"/>
     </row>
-    <row r="109" spans="2:8" ht="15.75" thickBot="1">
+    <row r="109" spans="2:8" ht="15" thickBot="1">
       <c r="C109" s="13"/>
       <c r="D109" s="12"/>
       <c r="E109" s="14"/>
@@ -2107,7 +2126,7 @@
       <c r="G109" s="14"/>
       <c r="H109" s="12"/>
     </row>
-    <row r="112" spans="2:8" ht="15.75" thickBot="1">
+    <row r="112" spans="2:8" ht="15" thickBot="1">
       <c r="B112" s="21">
         <v>9</v>
       </c>
@@ -2115,7 +2134,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="113" spans="2:8" ht="15.75" thickBot="1">
+    <row r="113" spans="2:8" ht="15" thickBot="1">
       <c r="C113" s="1" t="s">
         <v>0</v>
       </c>
@@ -2178,7 +2197,7 @@
       <c r="H116" s="8"/>
     </row>
     <row r="117" spans="2:8">
-      <c r="C117" s="3" t="s">
+      <c r="C117" s="23" t="s">
         <v>58</v>
       </c>
       <c r="D117" s="4" t="s">
@@ -2249,7 +2268,7 @@
       <c r="G122" s="10"/>
       <c r="H122" s="8"/>
     </row>
-    <row r="123" spans="2:8" ht="15.75" thickBot="1">
+    <row r="123" spans="2:8" ht="15" thickBot="1">
       <c r="C123" s="13"/>
       <c r="D123" s="12"/>
       <c r="E123" s="14"/>
@@ -2257,7 +2276,7 @@
       <c r="G123" s="14"/>
       <c r="H123" s="12"/>
     </row>
-    <row r="126" spans="2:8" ht="15.75" thickBot="1">
+    <row r="126" spans="2:8" ht="15" thickBot="1">
       <c r="B126" s="21">
         <v>10</v>
       </c>
@@ -2265,7 +2284,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="127" spans="2:8" ht="15.75" thickBot="1">
+    <row r="127" spans="2:8" ht="15" thickBot="1">
       <c r="C127" s="1" t="s">
         <v>0</v>
       </c>
@@ -2302,7 +2321,7 @@
       </c>
     </row>
     <row r="129" spans="2:8">
-      <c r="C129" s="3" t="s">
+      <c r="C129" s="23" t="s">
         <v>58</v>
       </c>
       <c r="D129" s="4" t="s">
@@ -2376,7 +2395,7 @@
       <c r="H134" s="8"/>
     </row>
     <row r="135" spans="2:8">
-      <c r="C135" s="3" t="s">
+      <c r="C135" s="23" t="s">
         <v>21</v>
       </c>
       <c r="D135" s="4" t="s">
@@ -2423,7 +2442,7 @@
       <c r="G138" s="10"/>
       <c r="H138" s="8"/>
     </row>
-    <row r="139" spans="2:8" ht="15.75" thickBot="1">
+    <row r="139" spans="2:8" ht="15" thickBot="1">
       <c r="C139" s="13"/>
       <c r="D139" s="12"/>
       <c r="E139" s="14"/>
@@ -2431,7 +2450,7 @@
       <c r="G139" s="14"/>
       <c r="H139" s="12"/>
     </row>
-    <row r="142" spans="2:8" ht="15.75" thickBot="1">
+    <row r="142" spans="2:8" ht="15" thickBot="1">
       <c r="B142" s="21">
         <v>11</v>
       </c>
@@ -2439,7 +2458,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="143" spans="2:8" ht="15.75" thickBot="1">
+    <row r="143" spans="2:8" ht="15" thickBot="1">
       <c r="C143" s="1" t="s">
         <v>0</v>
       </c>
@@ -2531,7 +2550,7 @@
       <c r="G149" s="5"/>
       <c r="H149" s="4"/>
     </row>
-    <row r="150" spans="2:8" ht="15.75" thickBot="1">
+    <row r="150" spans="2:8" ht="15" thickBot="1">
       <c r="C150" s="13"/>
       <c r="D150" s="12"/>
       <c r="E150" s="14"/>
@@ -2539,7 +2558,7 @@
       <c r="G150" s="14"/>
       <c r="H150" s="12"/>
     </row>
-    <row r="153" spans="2:8" ht="15.75" thickBot="1">
+    <row r="153" spans="2:8" ht="15" thickBot="1">
       <c r="B153" s="21">
         <v>12</v>
       </c>
@@ -2547,7 +2566,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="154" spans="2:8" ht="15.75" thickBot="1">
+    <row r="154" spans="2:8" ht="15" thickBot="1">
       <c r="C154" s="1" t="s">
         <v>0</v>
       </c>
@@ -2595,7 +2614,7 @@
       <c r="G156" s="5"/>
       <c r="H156" s="4"/>
     </row>
-    <row r="157" spans="2:8" ht="30">
+    <row r="157" spans="2:8" ht="28">
       <c r="C157" s="7" t="s">
         <v>100</v>
       </c>
@@ -2634,7 +2653,7 @@
       <c r="H159" s="8"/>
     </row>
     <row r="160" spans="2:8">
-      <c r="C160" s="3" t="s">
+      <c r="C160" s="23" t="s">
         <v>118</v>
       </c>
       <c r="D160" s="4" t="s">
@@ -2711,7 +2730,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="166" spans="2:8" ht="30">
+    <row r="166" spans="2:8" ht="28">
       <c r="C166" s="3" t="s">
         <v>116</v>
       </c>
@@ -2725,7 +2744,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="167" spans="2:8" ht="15.75" thickBot="1">
+    <row r="167" spans="2:8" ht="15" thickBot="1">
       <c r="C167" s="13"/>
       <c r="D167" s="12"/>
       <c r="E167" s="14"/>
@@ -2749,7 +2768,7 @@
       <c r="G169" s="25"/>
       <c r="H169" s="24"/>
     </row>
-    <row r="170" spans="2:8" ht="15.75" thickBot="1">
+    <row r="170" spans="2:8" ht="15" thickBot="1">
       <c r="B170" s="21">
         <v>11</v>
       </c>
@@ -2757,7 +2776,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="171" spans="2:8" ht="15.75" thickBot="1">
+    <row r="171" spans="2:8" ht="15" thickBot="1">
       <c r="C171" s="1" t="s">
         <v>0</v>
       </c>
@@ -2825,7 +2844,7 @@
       <c r="G175" s="5"/>
       <c r="H175" s="4"/>
     </row>
-    <row r="176" spans="2:8" ht="15.75" thickBot="1">
+    <row r="176" spans="2:8" ht="15" thickBot="1">
       <c r="C176" s="13"/>
       <c r="D176" s="12"/>
       <c r="E176" s="14"/>
@@ -2841,7 +2860,7 @@
       <c r="G177" s="25"/>
       <c r="H177" s="24"/>
     </row>
-    <row r="179" spans="2:8" ht="15.75" thickBot="1">
+    <row r="179" spans="2:8" ht="15" thickBot="1">
       <c r="B179" s="21">
         <v>13</v>
       </c>
@@ -2849,7 +2868,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="180" spans="2:8" ht="15.75" thickBot="1">
+    <row r="180" spans="2:8" ht="15" thickBot="1">
       <c r="C180" s="1" t="s">
         <v>0</v>
       </c>
@@ -2919,7 +2938,7 @@
       <c r="G184" s="5"/>
       <c r="H184" s="4"/>
     </row>
-    <row r="185" spans="2:8" ht="15.75" thickBot="1">
+    <row r="185" spans="2:8" ht="15" thickBot="1">
       <c r="C185" s="13"/>
       <c r="D185" s="12"/>
       <c r="E185" s="14"/>
@@ -2927,7 +2946,7 @@
       <c r="G185" s="14"/>
       <c r="H185" s="12"/>
     </row>
-    <row r="188" spans="2:8" ht="15.75" thickBot="1">
+    <row r="188" spans="2:8" ht="15" thickBot="1">
       <c r="B188" s="21">
         <v>14</v>
       </c>
@@ -2935,7 +2954,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="189" spans="2:8" ht="15.75" thickBot="1">
+    <row r="189" spans="2:8" ht="15" thickBot="1">
       <c r="C189" s="1" t="s">
         <v>0</v>
       </c>
@@ -3009,7 +3028,7 @@
       <c r="G193" s="5"/>
       <c r="H193" s="4"/>
     </row>
-    <row r="194" spans="3:8" ht="15.75" thickBot="1">
+    <row r="194" spans="3:8" ht="15" thickBot="1">
       <c r="C194" s="13"/>
       <c r="D194" s="12"/>
       <c r="E194" s="14"/>
@@ -3019,30 +3038,45 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>